<commit_message>
Updated XT60 PN and added render
</commit_message>
<xml_diff>
--- a/Hardware/Balance_Controller/EBOM_RevB.xlsx
+++ b/Hardware/Balance_Controller/EBOM_RevB.xlsx
@@ -193,7 +193,7 @@
     <t xml:space="preserve">Connector_AMASS:AMASS_XT60-F_1x02_P7.20mm_Vertical</t>
   </si>
   <si>
-    <t xml:space="preserve">XT60-F</t>
+    <t xml:space="preserve">XT60PB-F</t>
   </si>
   <si>
     <t xml:space="preserve">AMASS</t>
@@ -587,7 +587,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -615,11 +615,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -712,7 +707,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -796,10 +791,10 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.69"/>
@@ -1021,7 +1016,7 @@
       <c r="E10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="6" t="n">
         <v>3568</v>
       </c>
       <c r="G10" s="4" t="s">

</xml_diff>